<commit_message>
add new file and modified package name
</commit_message>
<xml_diff>
--- a/javabook-riskcontrol/src/main/resources/decision_table.xlsx
+++ b/javabook-riskcontrol/src/main/resources/decision_table.xlsx
@@ -9,7 +9,20 @@
   <sheets>
     <sheet name="Sheet1" sheetId="11" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,7 +38,7 @@
     <t>Import</t>
   </si>
   <si>
-    <t>cn.javabook.chapter05.entity.Coupon</t>
+    <t>cn.javabook.chapter12.entity.Coupon</t>
   </si>
   <si>
     <t>Variables</t>
@@ -864,7 +877,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{0720246A-E0CA-59F6-DB29-D865F5367147}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{E0FBB1A2-68AE-5636-BE01-4E661FE01DF9}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1138,7 +1151,7 @@
   <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="26" outlineLevelCol="7"/>

</xml_diff>